<commit_message>
caught some exceptions, and got rid of normed=True on histograms
</commit_message>
<xml_diff>
--- a/sheets/input/tests/Arnot_match _Pore_water_Dissolved_Water.xlsx
+++ b/sheets/input/tests/Arnot_match _Pore_water_Dissolved_Water.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_and_Time_Input" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="119">
   <si>
     <t xml:space="preserve">Sampling Variables Inputs</t>
   </si>
@@ -344,16 +344,16 @@
     <t xml:space="preserve">Coordinate 4</t>
   </si>
   <si>
-    <t xml:space="preserve">0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,0</t>
+    <t xml:space="preserve">0, 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0, 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30, 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30, 0</t>
   </si>
   <si>
     <t xml:space="preserve">Sites:</t>
@@ -365,7 +365,7 @@
     <t xml:space="preserve">(x,y) (meters)</t>
   </si>
   <si>
-    <t xml:space="preserve">10,10</t>
+    <t xml:space="preserve">10, 10</t>
   </si>
   <si>
     <t xml:space="preserve">Number of Regional Samples per Fish Population :</t>
@@ -401,20 +401,21 @@
     <t xml:space="preserve">Attraction Factor 1</t>
   </si>
   <si>
-    <t xml:space="preserve">0,10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,0</t>
+    <t xml:space="preserve">0, 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10, 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="167" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -555,7 +556,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -620,6 +621,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF200"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FFAFD095"/>
       </patternFill>
     </fill>
     <fill>
@@ -786,7 +793,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -811,7 +818,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -823,7 +830,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -843,7 +850,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -863,7 +870,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -935,7 +942,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -955,23 +962,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -983,7 +994,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1031,7 +1042,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1039,11 +1050,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1051,11 +1062,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="16" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1116,7 +1127,7 @@
       <rgbColor rgb="FFFAC090"/>
       <rgbColor rgb="FF538DD5"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF81D41A"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -1146,9 +1157,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1018800</xdr:colOff>
+      <xdr:colOff>1018440</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1158,7 +1169,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14044680" y="863280"/>
-          <a:ext cx="9471240" cy="7619040"/>
+          <a:ext cx="9470880" cy="7618680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1625,9 +1636,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3630960</xdr:colOff>
+      <xdr:colOff>3630600</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:rowOff>182520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1637,7 +1648,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12525120" y="699480"/>
-          <a:ext cx="3084480" cy="995760"/>
+          <a:ext cx="3084120" cy="995400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1848,9 +1859,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2331360</xdr:colOff>
+      <xdr:colOff>2331000</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1864,7 +1875,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16676280" y="10278720"/>
-          <a:ext cx="2331360" cy="735480"/>
+          <a:ext cx="2331000" cy="735120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1885,9 +1896,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4592880</xdr:colOff>
+      <xdr:colOff>4592520</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1897,7 +1908,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11825640" y="2007000"/>
-          <a:ext cx="9443520" cy="3201120"/>
+          <a:ext cx="9443160" cy="3200760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2364,9 +2375,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>786240</xdr:colOff>
+      <xdr:colOff>785880</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2376,7 +2387,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16928640" y="190440"/>
-          <a:ext cx="3603240" cy="761040"/>
+          <a:ext cx="3602880" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2506,9 +2517,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1132920</xdr:colOff>
+      <xdr:colOff>1132560</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2518,7 +2529,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14774760" y="1714680"/>
-          <a:ext cx="2930760" cy="760680"/>
+          <a:ext cx="2930400" cy="760320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2590,9 +2601,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>643680</xdr:colOff>
+      <xdr:colOff>643320</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2602,7 +2613,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10537200" y="2522160"/>
-          <a:ext cx="9088200" cy="3567960"/>
+          <a:ext cx="9087840" cy="3567600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3130,9 +3141,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>151200</xdr:colOff>
+      <xdr:colOff>150840</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3142,7 +3153,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10606320" y="674280"/>
-          <a:ext cx="4075560" cy="949320"/>
+          <a:ext cx="4075200" cy="948960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3249,9 +3260,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3566520</xdr:colOff>
+      <xdr:colOff>3566160</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3261,7 +3272,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4629240" y="4925160"/>
-          <a:ext cx="5158080" cy="761040"/>
+          <a:ext cx="5157720" cy="760680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3363,9 +3374,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2593080</xdr:colOff>
+      <xdr:colOff>2592720</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3375,7 +3386,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16049880" y="5488560"/>
-          <a:ext cx="4331160" cy="341280"/>
+          <a:ext cx="4330800" cy="340920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3447,9 +3458,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5383800</xdr:colOff>
+      <xdr:colOff>5383440</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>138240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3459,7 +3470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9213840" y="76320"/>
-          <a:ext cx="5256720" cy="1497240"/>
+          <a:ext cx="5256360" cy="1496880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3661,9 +3672,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6884280</xdr:colOff>
+      <xdr:colOff>6883920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>87840</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3673,7 +3684,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10153440" y="2298600"/>
-          <a:ext cx="5817600" cy="659160"/>
+          <a:ext cx="5817240" cy="658800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3780,9 +3791,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3792,7 +3803,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11960640" y="241200"/>
-          <a:ext cx="5136120" cy="392400"/>
+          <a:ext cx="5135760" cy="392040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3904,9 +3915,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>100440</xdr:colOff>
+      <xdr:colOff>100080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3916,7 +3927,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12062160" y="1295280"/>
-          <a:ext cx="3862440" cy="417960"/>
+          <a:ext cx="3862080" cy="417600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3973,9 +3984,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>469080</xdr:colOff>
+      <xdr:colOff>468720</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3985,7 +3996,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12087720" y="2158560"/>
-          <a:ext cx="5225040" cy="697680"/>
+          <a:ext cx="5224680" cy="697320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4047,9 +4058,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>278280</xdr:colOff>
+      <xdr:colOff>277920</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>164160</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4059,7 +4070,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13899240" y="761760"/>
-          <a:ext cx="6530760" cy="5879160"/>
+          <a:ext cx="6530400" cy="5878800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4175,7 +4186,7 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -4688,7 +4699,7 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -4855,10 +4866,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4883,29 +4894,35 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="41" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="43" t="n">
+      <c r="B6" s="44" t="n">
         <v>2.23E-005</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="41" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="44" t="n">
+      <c r="B7" s="45" t="n">
         <v>0.0002257</v>
       </c>
     </row>
@@ -4927,7 +4944,7 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -4946,28 +4963,28 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="47" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4975,25 +4992,25 @@
       <c r="A2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>72</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="49" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="49" t="s">
         <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="49" t="s">
         <v>71</v>
       </c>
     </row>
@@ -5001,25 +5018,25 @@
       <c r="A3" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="49" t="n">
+      <c r="B3" s="50" t="n">
         <v>0.0004</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="49" t="n">
+      <c r="D3" s="50" t="n">
         <v>0.00011</v>
       </c>
       <c r="E3" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="49" t="n">
+      <c r="F3" s="50" t="n">
         <v>5.7E-008</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="49" t="n">
+      <c r="H3" s="50" t="n">
         <v>0.08</v>
       </c>
     </row>
@@ -5033,19 +5050,19 @@
       <c r="C4" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="48" t="n">
+      <c r="D4" s="49" t="n">
         <v>0.013</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="48" t="n">
+      <c r="F4" s="49" t="n">
         <v>0.012</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H4" s="48"/>
+      <c r="H4" s="49"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
@@ -5055,15 +5072,15 @@
       <c r="C5" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="H5" s="49"/>
+      <c r="H5" s="50"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
@@ -5080,7 +5097,7 @@
         <v>80</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="51" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5088,7 +5105,7 @@
       <c r="A7" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="51"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="28" t="s">
         <v>81</v>
       </c>
@@ -5097,13 +5114,13 @@
         <v>81</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="52"/>
+      <c r="G7" s="53"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="51"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="28" t="s">
         <v>82</v>
       </c>
@@ -5117,7 +5134,7 @@
       <c r="A9" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="48"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="28" t="s">
         <v>83</v>
       </c>
@@ -5131,7 +5148,7 @@
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="53"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="1" t="s">
         <v>84</v>
       </c>
@@ -5145,34 +5162,34 @@
       <c r="A11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="48"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="54"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="54"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="54" t="n">
+      <c r="B12" s="55" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="56" t="n">
+      <c r="D12" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="57" t="n">
+      <c r="F12" s="58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5181,14 +5198,14 @@
       <c r="B13" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="50" t="s">
+      <c r="E13" s="59"/>
+      <c r="F13" s="51" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5198,7 +5215,7 @@
       <c r="C14" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="49" t="s">
         <v>86</v>
       </c>
     </row>
@@ -5208,7 +5225,7 @@
       <c r="C15" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="49" t="n">
+      <c r="D15" s="50" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -5218,7 +5235,7 @@
       <c r="C16" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="48" t="n">
+      <c r="D16" s="49" t="n">
         <v>0.021</v>
       </c>
     </row>
@@ -5228,7 +5245,7 @@
       <c r="C17" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="48"/>
+      <c r="D17" s="49"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
@@ -5278,15 +5295,15 @@
       <c r="C23" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="54"/>
+      <c r="D23" s="55"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="56" t="n">
+      <c r="D24" s="57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5327,56 +5344,56 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="61" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="61"/>
+      <c r="B2" s="62"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="61" t="n">
+      <c r="B3" s="62" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="61" t="n">
+      <c r="B4" s="62" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="61" t="n">
+      <c r="B5" s="62" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="61" t="n">
+      <c r="B6" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="B7" s="61" t="n">
+      <c r="B7" s="62" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="32"/>
@@ -5384,72 +5401,72 @@
       <c r="E7" s="32"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="61" t="n">
+      <c r="B8" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="61" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="61"/>
+      <c r="B10" s="62"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="61" t="n">
+      <c r="B11" s="62" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="61" t="n">
+      <c r="B12" s="62" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="61" t="n">
+      <c r="B13" s="62" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="61" t="n">
+      <c r="B14" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="61" t="n">
+      <c r="B15" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="61" t="n">
+      <c r="B16" s="62" t="n">
         <v>0</v>
       </c>
       <c r="H16" s="32"/>
@@ -5457,56 +5474,56 @@
       <c r="J16" s="32"/>
     </row>
     <row r="17" customFormat="false" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="61" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="61"/>
+      <c r="B18" s="62"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="61" t="n">
+      <c r="B19" s="62" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="61" t="n">
+      <c r="B20" s="62" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="61" t="s">
+      <c r="A21" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="61" t="n">
+      <c r="B21" s="62" t="n">
         <v>0.7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="61" t="n">
+      <c r="B22" s="62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="61" t="n">
+      <c r="B23" s="62" t="n">
         <v>0.1</v>
       </c>
       <c r="H23" s="32"/>
@@ -5514,10 +5531,10 @@
       <c r="J23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="61" t="s">
+      <c r="A24" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="61" t="n">
+      <c r="B24" s="62" t="n">
         <v>0</v>
       </c>
       <c r="H24" s="32"/>
@@ -6086,16 +6103,16 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="63" t="n">
+      <c r="B2" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="64" t="n">
+      <c r="C2" s="65" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="64" t="n">
+      <c r="D2" s="65" t="n">
         <v>1</v>
       </c>
       <c r="FU2" s="32"/>
@@ -6136,8 +6153,8 @@
   </sheetPr>
   <dimension ref="A1:AW100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6551,9 +6568,9 @@
       <c r="H37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="65"/>
-      <c r="B38" s="65"/>
-      <c r="C38" s="65"/>
+      <c r="A38" s="66"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
       <c r="D38" s="32"/>
       <c r="E38" s="32"/>
       <c r="F38" s="32"/>
@@ -6561,16 +6578,16 @@
       <c r="H38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="66" t="n">
+      <c r="B39" s="67" t="n">
         <v>40</v>
       </c>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="66" t="s">
+      <c r="D39" s="67" t="s">
         <v>108</v>
       </c>
       <c r="E39" s="32"/>
@@ -6579,49 +6596,49 @@
       <c r="H39" s="32"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="63" t="s">
+      <c r="A40" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="63" t="s">
+      <c r="C40" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="67" t="s">
+      <c r="D40" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="67" t="s">
+      <c r="E40" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="F40" s="67" t="s">
+      <c r="F40" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="G40" s="67" t="s">
+      <c r="G40" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="H40" s="68"/>
+      <c r="H40" s="69"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="63" t="s">
+      <c r="A41" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="63" t="n">
+      <c r="C41" s="64" t="n">
         <v>1</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D41" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="63" t="s">
+      <c r="E41" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="F41" s="63" t="s">
+      <c r="F41" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="G41" s="63" t="s">
+      <c r="G41" s="64" t="s">
         <v>118</v>
       </c>
       <c r="H41" s="32"/>
@@ -6630,182 +6647,182 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="63"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
+      <c r="A42" s="64"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
       <c r="H42" s="32"/>
       <c r="AW42" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="64"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="64"/>
+      <c r="A43" s="65"/>
+      <c r="B43" s="65"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
       <c r="AW43" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="64"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="64"/>
+      <c r="A44" s="65"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="65"/>
       <c r="AW44" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="64"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
+      <c r="A45" s="65"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="65"/>
       <c r="AW45" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
+      <c r="A46" s="65"/>
+      <c r="B46" s="65"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="65"/>
       <c r="AW46" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="64"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="64"/>
+      <c r="A47" s="65"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="65"/>
       <c r="AW47" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="64"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="64"/>
+      <c r="A48" s="65"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="65"/>
       <c r="AW48" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="64"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
+      <c r="A49" s="65"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="65"/>
       <c r="AW49" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="64"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="64"/>
+      <c r="A50" s="65"/>
+      <c r="B50" s="65"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="65"/>
       <c r="AW50" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="64"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
+      <c r="A51" s="65"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="65"/>
+      <c r="E51" s="65"/>
+      <c r="F51" s="65"/>
+      <c r="G51" s="65"/>
       <c r="AW51" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="64"/>
-      <c r="B52" s="64"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
+      <c r="A52" s="65"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65"/>
+      <c r="G52" s="65"/>
       <c r="AW52" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="64"/>
-      <c r="B53" s="64"/>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="64"/>
+      <c r="A53" s="65"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="65"/>
+      <c r="F53" s="65"/>
+      <c r="G53" s="65"/>
       <c r="AW53" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="64"/>
-      <c r="B54" s="64"/>
-      <c r="C54" s="64"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="64"/>
+      <c r="A54" s="65"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="65"/>
+      <c r="G54" s="65"/>
       <c r="AW54" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="64"/>
-      <c r="B55" s="64"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="64"/>
-      <c r="E55" s="64"/>
-      <c r="F55" s="64"/>
-      <c r="G55" s="64"/>
+      <c r="A55" s="65"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="65"/>
+      <c r="F55" s="65"/>
+      <c r="G55" s="65"/>
       <c r="AW55" s="0" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="64"/>
-      <c r="B56" s="64"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="64"/>
+      <c r="A56" s="65"/>
+      <c r="B56" s="65"/>
+      <c r="C56" s="65"/>
+      <c r="D56" s="65"/>
+      <c r="E56" s="65"/>
+      <c r="F56" s="65"/>
+      <c r="G56" s="65"/>
       <c r="AW56" s="0" t="s">
         <v>62</v>
       </c>

</xml_diff>